<commit_message>
Created Workbooks which include sheets for each protein, either eith their GOs, or with their partners. The output html includes collapsable tables
</commit_message>
<xml_diff>
--- a/Project_Datasets/Go_terms_OI.xlsx
+++ b/Project_Datasets/Go_terms_OI.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>GO:0000077</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>GO:0008630</t>
+  </si>
+  <si>
+    <t>GO:0005739</t>
+  </si>
+  <si>
+    <t>GO:0016020</t>
   </si>
 </sst>
 </file>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A89"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +446,18 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>